<commit_message>
cleanup in file with topics
</commit_message>
<xml_diff>
--- a/doc/topics.xlsx
+++ b/doc/topics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" state="visible" r:id="rId2"/>
@@ -52,9 +52,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">reopen</t>
-  </si>
-  <si>
     <t xml:space="preserve">filtry do pobierania orderów</t>
   </si>
   <si>
@@ -75,7 +72,8 @@
 Kuba: Bedziemy jednak potrzebowac uslug 
 a) do pobierania orderow po statusie – zaakceptowane bez numeru protokolu – do wstawiania numerow protokolu przez prezesa (formularz ID:7) 
 b) do wybierania orderow po przypisaniu – aby modyfikacje na status wykonane mogl zrobic tylko inzynier (formularz ID:5) ktory nad danym zleceniem pracowal
-</t>
+Łukasz:
+Dodane</t>
   </si>
   <si>
     <t xml:space="preserve">po co tabela kontakt</t>
@@ -91,9 +89,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">open</t>
-  </si>
-  <si>
     <t xml:space="preserve">pole Version w orderze</t>
   </si>
   <si>
@@ -101,7 +96,10 @@
 Czemu WO ma Version? czy to jest trudny latwy? jesli nie to tego brakuje,
 Łukasz:
 Żeby łatwiej przeglądać historię. Teoretycznie data LAST_MOD wystarczy, ale tak od razu jest info, ile razy workordr był zmieniany. Można usunąć.
-Kuba: do usuniecia – nie potrzebne wg mnie</t>
+Kuba: do usuniecia – nie potrzebne wg mnie
+Łukasz:
+Usunięte
+</t>
   </si>
   <si>
     <t xml:space="preserve">brak współczynnika pracochłonnosci</t>
@@ -135,7 +133,10 @@
 Jasne, tabele dodam. Tylko czy jak pojawi się nowy stopień skomplikowanie, np. łatwe albo bardzo trudne to nie trzeba modyfikować kodu ? Gdyby zamiast COMPLEXITY_STANDARD, COMPLEXITY_COMPLEX zrobić jedną kolumnę z wartościami słownikowymi takimi jak w WO to będzie po prostu złączenie. A obecnie trzeba będzie  robić CASE'a w triggerze i dla nowych trudności dodawać przypadek.
 Łukasz:
 To pole LOCALIZATION, to jest to samo co w PERSON pole zawierające lokalizację, czyli miasto gdzie jest biuro?
-Kuba: To jest lokalizacja biura, ktore wykona to zlecenie – ale tu bedzie pytanie do inwestora, czy takie zlecenie ma szanse przejsc do innego biura</t>
+Kuba: To jest lokalizacja biura, ktore wykona to zlecenie – ale tu bedzie pytanie do inwestora, czy takie zlecenie ma szanse przejsc do innego biura
+Łukasz:
+Gotowe
+</t>
   </si>
   <si>
     <t xml:space="preserve">brak pól w order</t>
@@ -149,7 +150,14 @@
 Przedstawiciel inwestora to relacja do Person, gdzie person ma specjalny typ ?
 Adres lokalizacji już jest – referencja z ADDRESS do WORK_ORDER.
 Rekord testowy dodam. Ogólnie trochę jeszcze po zmieniałem, bo były błędy.
-Kuba: tak to moze byc specjalna rola w PERSON, ktora nie bedzie miec konta w account</t>
+Kuba: tak to moze byc specjalna rola w PERSON, ktora nie bedzie miec konta w account
+Łukasz:
+Tu mi się trochę pamięć urywa.
+Widzę, że wykomentowałem tabelę ACCOUNT a dane do logowania przeniosłem do  PERSON. Dodałem rolę dla przedstawiciela klienta. W tabeli WORK_ORDER jest description, więc chyba gotowe.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open</t>
   </si>
   <si>
     <t xml:space="preserve">Spisanie statusow WO do excel</t>
@@ -164,16 +172,25 @@
     <t xml:space="preserve">do przygotowania spec I implementacja</t>
   </si>
   <si>
+    <t xml:space="preserve">reopen</t>
+  </si>
+  <si>
     <t xml:space="preserve">adres</t>
   </si>
   <si>
-    <t xml:space="preserve">adres to text zdefiniowany poza WO – relacja jeden do wielu – kopiowanie adresow miedzy wo</t>
+    <t xml:space="preserve">adres to text zdefiniowany poza WO – relacja jeden do wielu – kopiowanie adresow miedzy wo
+Łukasz:
+Potwierdz, że obecny model danych do adresu jest ok ???
+</t>
   </si>
   <si>
     <t xml:space="preserve">externalID</t>
   </si>
   <si>
-    <t xml:space="preserve">numer WO czyli externalID jest opcjonalny I moze sie powtarzac</t>
+    <t xml:space="preserve">numer WO czyli externalID jest opcjonalny I moze sie powtarzac
+Łukasz:
+Pole dodane wraz z wyszukiwaniem po nim
+</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -307,7 +324,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -352,14 +369,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF990000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF990000"/>
+      <color rgb="FF999999"/>
       <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -434,7 +444,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -460,22 +470,30 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -506,7 +524,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF990000"/>
+      <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -566,21 +584,21 @@
   </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="94.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="94.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -615,14 +633,14 @@
       <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="156.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,24 +651,24 @@
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="118.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="132.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,10 +679,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,100 +693,100 @@
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="215.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="196.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="147.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="167.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>22</v>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="0" t="s">
+      <c r="B10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="B11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="50.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="50.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="4" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -783,34 +801,34 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.0357142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="39.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="39.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="12" t="s">
         <v>35</v>
       </c>
     </row>
@@ -821,13 +839,13 @@
       <c r="B2" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -838,13 +856,13 @@
       <c r="B3" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="13" t="s">
         <v>41</v>
       </c>
     </row>
@@ -855,13 +873,13 @@
       <c r="B4" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -872,13 +890,13 @@
       <c r="B5" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -887,13 +905,13 @@
       <c r="B6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -902,13 +920,13 @@
       <c r="B7" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -917,13 +935,13 @@
       <c r="B8" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="13" t="s">
         <v>51</v>
       </c>
     </row>
@@ -934,13 +952,13 @@
       <c r="B9" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="13" t="s">
         <v>53</v>
       </c>
     </row>
@@ -951,13 +969,13 @@
       <c r="B10" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="13" t="s">
         <v>55</v>
       </c>
     </row>
@@ -968,13 +986,13 @@
       <c r="B11" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -983,13 +1001,13 @@
       <c r="B12" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -998,13 +1016,13 @@
       <c r="B13" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -1013,13 +1031,13 @@
       <c r="B14" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -1028,39 +1046,39 @@
       <c r="B15" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="12"/>
+      <c r="C17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="12"/>
+      <c r="C19" s="14"/>
     </row>
     <row r="20" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="14" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Additional meta colums for WORK_ORDER, roles consideration
</commit_message>
<xml_diff>
--- a/doc/topics.xlsx
+++ b/doc/topics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -163,25 +163,69 @@
     <t xml:space="preserve">Spisanie statusow WO do excel</t>
   </si>
   <si>
-    <t xml:space="preserve">Do weryfikacji czy trzeba dorobic status dla protokolu? s</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Do weryfikacji czy trzeba dorobic status dla protokolu? 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Kuba: wyjdzie podczas implementacji, na razie zakladamy ze logika bedzie tylko w GUI wydaje sie to prostrze
+OTWARTE – wpisano do systemu
+PRZYPISANE – Przez operatora, rownież po braku akceptacji
+ZAKONCZONE – Z punktu widzenia inzyniera
+WYDANE- Dokumentacja poszla do zleceniodowcy
+ZAAKCEPTOWANE – Przez Zleceniodawce
+ZAMKNIETE – rozliczono protokol
+ZAWIESZONE – Wstrzymano prace</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">nowe typy komentarzy – meta-danych</t>
   </si>
   <si>
-    <t xml:space="preserve">do przygotowania spec I implementacja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reopen</t>
+    <t xml:space="preserve">do przygotowania spec I implementacja
+Kuba: Przygotowalem takie pola:
+ MD_CAPEX VARCHAR(255), --MD stands for META-DATA
+    MD_BUILDING_TYPE VARCHAR(255),
+    MD_CONSTRUCTION_CATEGORY VARCHAR(255),</t>
   </si>
   <si>
     <t xml:space="preserve">adres</t>
   </si>
   <si>
-    <t xml:space="preserve">adres to text zdefiniowany poza WO – relacja jeden do wielu – kopiowanie adresow miedzy wo
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB2B2B2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">adres to text zdefiniowany poza WO – relacja jeden do wielu – kopiowanie adresow miedzy wo
 Łukasz:
 Potwierdz, że obecny model danych do adresu jest ok ???
+ Kuba:
 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFB2B2B2"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Potwierdzam - ADDRESS_TEXT VARCHAR(100)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">externalID</t>
@@ -193,6 +237,33 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">problem z rolami</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Role – Zdefiniowalimsy 4 role uzytkonikow (VE nie jest uzytkownikem systemu)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Prezes (edycja daty) - PR
+Administrator/Operator - OP
+Kierownik - MG
+Projektant/Inzynier - EG
+Role te nie sa do konca hierarchiczne tj nie ma dziedziczenia np. Administrator nie jest kierownikiem. Jesli wiec mamy relacje 1do1 miedzy osoba a rola, to nie mozemy miec osoby w dwoch rolach np. Musimy dokonac zalozenia ze kierownik jest tez inzynierem jako hardcode oraz ze operator ma badz nie ma w zaleznosci od wymagan uprawnienia kierownika… Dodatkowo musimy dodac modul sprawdzania ACL w Backendzie – np. Zeby nikt znajacy token I zalogowany nie mogl generowac raportow</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
@@ -214,16 +285,16 @@
     <t xml:space="preserve">Wprowadzanie WO</t>
   </si>
   <si>
-    <t xml:space="preserve">Operator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W przypadku inne prezes wystepuje w roli operator I wprowadza cene z palca</t>
+    <t xml:space="preserve">PR+OP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W przypadku typu zlecenia “INNE” prezes wystepuje w roli operator I wprowadza cene z palca</t>
   </si>
   <si>
     <t xml:space="preserve">Edycja WO / Zmiana Statusu WO</t>
   </si>
   <si>
-    <t xml:space="preserve">Ceny widoczne, mozliwe do modyfikacji  tylko WO innych niz inne, widocznosc tylko dla Prezes</t>
+    <t xml:space="preserve">Ceny widoczne, mozliwe do modyfikacji  tylko WO innych niz “INNE”, widocznosc “INNYCH” tylko dla Prezes</t>
   </si>
   <si>
     <t xml:space="preserve">Przypisanie WO do pracownika/pracownikow</t>
@@ -257,19 +328,16 @@
     <t xml:space="preserve">Zakonczenie pracy nad przypisanym WO</t>
   </si>
   <si>
-    <t xml:space="preserve">Inzynier</t>
+    <t xml:space="preserve">EN</t>
   </si>
   <si>
     <t xml:space="preserve">Zmiana kwalifikacji trudne/latwe</t>
   </si>
   <si>
-    <t xml:space="preserve">Kierownik</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nadawanie numeru protokolu WO do rozliczenia</t>
   </si>
   <si>
-    <t xml:space="preserve">Prezes</t>
+    <t xml:space="preserve">PR</t>
   </si>
   <si>
     <t xml:space="preserve">Usluga daje wszystkie zaakceptowane nierozliczone WO, ale mozna je oznaczyc na ekranie I tylko zaznaczonym przypisac numer protokolu. Do numeru dodajemy suffix /ID_ZLECAJACEGO</t>
@@ -291,6 +359,9 @@
   </si>
   <si>
     <t xml:space="preserve">Wprowadzanie nowych typow WO wraz z parametrami – domyslna cena, czasochlonnosc per lokalizacja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesli WO jest kontynuacja prac dla tej samej stacji nalezy zaimplementowac autouzupelnianie</t>
   </si>
   <si>
     <t xml:space="preserve">Wprowadzanie nowych pracownikow</t>
@@ -324,7 +395,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -375,6 +446,17 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFB2B2B2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -444,7 +526,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -489,16 +571,28 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -582,23 +676,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="94.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="93.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -727,7 +821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="113.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
@@ -737,56 +831,70 @@
       <c r="C10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+    <row r="11" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="113.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="50.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="50.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C14" s="0" t="s">
         <v>30</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -801,52 +909,51 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="39.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.23"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="39.280612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="25.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E1" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="48.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="15" t="s">
         <v>39</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -854,16 +961,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>41</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="87.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -871,214 +978,216 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="13"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="13"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="13" t="s">
+      <c r="C14" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="13"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="C15" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="D15" s="15" t="s">
         <v>64</v>
       </c>
+      <c r="E15" s="15" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="14"/>
+      <c r="C17" s="17"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="14"/>
+      <c r="C19" s="17"/>
     </row>
     <row r="20" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>65</v>
+      <c r="C20" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
small info added, draft corrected
</commit_message>
<xml_diff>
--- a/doc/topics.xlsx
+++ b/doc/topics.xlsx
@@ -297,8 +297,9 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">3. Oddzielne API do przypisania z jednej osoby na druga, oddzielne do przypisania drugiej osobie nie kasujace poprzedniego przypisania</t>
+      <t xml:space="preserve">3. Nie potrzebne jest iddzielne API do przypisania z jednej osoby na druga, oddzielne do przypisania drugiej osobie nie kasujace poprzedniego przypisania – front zadba zeby skasowac relacje jesli jest to potrzebne</t>
     </r>
   </si>
   <si>
@@ -387,7 +388,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -457,11 +458,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -686,10 +682,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="88.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="88.015306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,17 +944,17 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="37.2602040816326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>